<commit_message>
create scheme + write queries
</commit_message>
<xml_diff>
--- a/data/managers.xlsx
+++ b/data/managers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD80AA90-8E6D-46ED-831B-BF166340C3D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48443773-9959-4C0A-ABEF-21912F1AE030}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -776,6 +776,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -805,10 +808,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1097,7 +1101,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1110,7 +1114,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">

</xml_diff>